<commit_message>
add team name and repo
</commit_message>
<xml_diff>
--- a/Security Task Team Information.xlsx
+++ b/Security Task Team Information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VICTUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D07611-060B-4F02-845B-507462F4CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A9AB84-0C5F-4683-B13E-EBB31A213EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>لينك ال repo</t>
   </si>
@@ -56,32 +56,38 @@
     <t>اسم الفرد السادس</t>
   </si>
   <si>
-    <t xml:space="preserve">احمد خالد محمد </t>
-  </si>
-  <si>
-    <t>إسماعيل عبدالله عزب</t>
-  </si>
-  <si>
-    <t>حنان احمد مصطفي</t>
-  </si>
-  <si>
-    <t>روان زينهم عبدالعزيز</t>
-  </si>
-  <si>
-    <t>عبدالله محمد خالد عبدالباسط</t>
-  </si>
-  <si>
-    <t>عبدالرحمن علاء الدين عبدالمنعم</t>
-  </si>
-  <si>
-    <t>https://github.com/AbdallahHikal/Steganography.git</t>
+    <t>https://github.com/Momen-magdy/websiteforsianna</t>
+  </si>
+  <si>
+    <t>مؤمن مجدى عبدالعزيز</t>
+  </si>
+  <si>
+    <t>احمد بلال عبدالمجيد</t>
+  </si>
+  <si>
+    <t>احمد اسماعيل دياب</t>
+  </si>
+  <si>
+    <t>محمود محمد فؤاد</t>
+  </si>
+  <si>
+    <t>محمود محمد ابراهيم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عمر محمد محمد </t>
+  </si>
+  <si>
+    <t>اسم الفرد السابع</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احمد يحى محمد </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -91,12 +97,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -133,13 +133,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -366,21 +365,22 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="C9:F9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" customWidth="1"/>
+    <col min="2" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,32 +399,37 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>